<commit_message>
Added Bivariate analysis code & also update the Analysis Approach and other details in code file
</commit_message>
<xml_diff>
--- a/Data_Dictionary.xlsx
+++ b/Data_Dictionary.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vikrampawar/VikramPawar/Self_Learning/Certifications_Courses/IIITB_AI_ML_Course/Case_Studies/LendingClub_Case_Study/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1D9382E8-F58C-8E4F-8384-199E5FF8EC44}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D06BD21F-3ADD-544E-938A-9DF2B40F9276}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16000" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="LoanStats" sheetId="3" r:id="rId1"/>
@@ -1860,9 +1860,9 @@
   </sheetPr>
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" sqref="A1:XFD1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3004,11 +3004,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{772E8740-F1F1-5C4E-B137-1D109ADBDF19}">
-  <sheetPr filterMode="1"/>
   <dimension ref="A1:K118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" workbookViewId="0">
-      <selection activeCell="C87" sqref="C87"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="31.33203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -3035,7 +3034,7 @@
         <v>252</v>
       </c>
     </row>
-    <row r="2" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A2" s="9" t="s">
         <v>229</v>
       </c>
@@ -3053,7 +3052,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A3" s="9" t="s">
         <v>233</v>
       </c>
@@ -3089,7 +3088,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:7" s="5" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" s="5" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="9" t="s">
         <v>223</v>
       </c>
@@ -3125,7 +3124,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="7" spans="1:7" s="4" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:7" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A7" s="7" t="s">
         <v>191</v>
       </c>
@@ -3143,7 +3142,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="8" spans="1:7" s="4" customFormat="1" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:7" s="4" customFormat="1" ht="32" x14ac:dyDescent="0.2">
       <c r="A8" s="7" t="s">
         <v>189</v>
       </c>
@@ -3161,7 +3160,7 @@
         <v>9</v>
       </c>
     </row>
-    <row r="9" spans="1:7" s="4" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="9" t="s">
         <v>108</v>
       </c>
@@ -3179,7 +3178,7 @@
         <v>154</v>
       </c>
     </row>
-    <row r="10" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="9" t="s">
         <v>234</v>
       </c>
@@ -3197,7 +3196,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="11" spans="1:7" s="5" customFormat="1" ht="14" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:7" s="5" customFormat="1" ht="14" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="9" t="s">
         <v>235</v>
       </c>
@@ -3215,7 +3214,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="12" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="9" t="s">
         <v>99</v>
       </c>
@@ -3233,7 +3232,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="7" t="s">
         <v>165</v>
       </c>
@@ -3251,7 +3250,7 @@
         <v>232</v>
       </c>
     </row>
-    <row r="14" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="3" t="s">
         <v>100</v>
       </c>
@@ -3287,7 +3286,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="16" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A16" s="9" t="s">
         <v>236</v>
       </c>
@@ -3305,7 +3304,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="17" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A17" s="3" t="s">
         <v>17</v>
       </c>
@@ -3341,7 +3340,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="19" spans="1:7" s="4" customFormat="1" ht="48" hidden="1" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:7" s="4" customFormat="1" ht="48" x14ac:dyDescent="0.2">
       <c r="A19" s="7" t="s">
         <v>192</v>
       </c>
@@ -3413,7 +3412,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="23" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A23" s="7" t="s">
         <v>25</v>
       </c>
@@ -3431,7 +3430,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="24" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A24" s="7" t="s">
         <v>24</v>
       </c>
@@ -3467,7 +3466,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A26" s="3" t="s">
         <v>4</v>
       </c>
@@ -3521,7 +3520,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="29" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A29" s="3" t="s">
         <v>0</v>
       </c>
@@ -3539,7 +3538,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="30" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A30" s="9" t="s">
         <v>215</v>
       </c>
@@ -3557,7 +3556,7 @@
         <v>97</v>
       </c>
     </row>
-    <row r="31" spans="1:7" s="4" customFormat="1" ht="18" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:7" s="4" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="3" t="s">
         <v>34</v>
       </c>
@@ -3572,7 +3571,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="32" spans="1:7" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:7" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A32" s="9" t="s">
         <v>225</v>
       </c>
@@ -3587,7 +3586,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="33" spans="1:11" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A33" s="9" t="s">
         <v>227</v>
       </c>
@@ -3664,7 +3663,7 @@
       <c r="I37" s="10"/>
       <c r="J37" s="11"/>
     </row>
-    <row r="38" spans="1:11" s="4" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:11" s="4" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A38" s="3" t="s">
         <v>45</v>
       </c>
@@ -3679,7 +3678,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="39" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A39" s="7" t="s">
         <v>46</v>
       </c>
@@ -3694,7 +3693,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="40" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A40" s="7" t="s">
         <v>47</v>
       </c>
@@ -3709,7 +3708,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="41" spans="1:11" ht="16" hidden="1" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:11" ht="16" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="3" t="s">
         <v>43</v>
       </c>
@@ -3724,7 +3723,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="42" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A42" s="3" t="s">
         <v>42</v>
       </c>
@@ -3769,7 +3768,7 @@
         <v>Present</v>
       </c>
     </row>
-    <row r="45" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A45" s="9" t="s">
         <v>221</v>
       </c>
@@ -3784,7 +3783,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="46" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A46" s="3" t="s">
         <v>1</v>
       </c>
@@ -3802,7 +3801,7 @@
       <c r="J46" s="11"/>
       <c r="K46" s="11"/>
     </row>
-    <row r="47" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A47" s="9" t="s">
         <v>237</v>
       </c>
@@ -3820,7 +3819,7 @@
       <c r="J47" s="11"/>
       <c r="K47" s="11"/>
     </row>
-    <row r="48" spans="1:11" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:11" ht="16" x14ac:dyDescent="0.2">
       <c r="A48" s="9" t="s">
         <v>118</v>
       </c>
@@ -3838,7 +3837,7 @@
       <c r="J48" s="11"/>
       <c r="K48" s="11"/>
     </row>
-    <row r="49" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A49" s="9" t="s">
         <v>119</v>
       </c>
@@ -3853,7 +3852,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="50" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A50" s="9" t="s">
         <v>105</v>
       </c>
@@ -3868,7 +3867,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="51" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A51" s="9" t="s">
         <v>238</v>
       </c>
@@ -3898,7 +3897,7 @@
         <v>Present</v>
       </c>
     </row>
-    <row r="53" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A53" s="8" t="s">
         <v>102</v>
       </c>
@@ -3913,7 +3912,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="54" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A54" s="3" t="s">
         <v>28</v>
       </c>
@@ -3928,7 +3927,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="55" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A55" s="9" t="s">
         <v>211</v>
       </c>
@@ -3943,7 +3942,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="56" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A56" s="9" t="s">
         <v>239</v>
       </c>
@@ -3958,7 +3957,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="57" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A57" s="8" t="s">
         <v>240</v>
       </c>
@@ -3973,7 +3972,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="58" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A58" s="9" t="s">
         <v>242</v>
       </c>
@@ -3988,7 +3987,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="59" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A59" s="9" t="s">
         <v>243</v>
       </c>
@@ -4003,7 +4002,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="60" spans="1:4" s="6" customFormat="1" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:4" s="6" customFormat="1" ht="16" x14ac:dyDescent="0.2">
       <c r="A60" s="3" t="s">
         <v>44</v>
       </c>
@@ -4018,7 +4017,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="61" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A61" s="9" t="s">
         <v>98</v>
       </c>
@@ -4033,7 +4032,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="62" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A62" s="9" t="s">
         <v>110</v>
       </c>
@@ -4048,7 +4047,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="63" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A63" s="9" t="s">
         <v>117</v>
       </c>
@@ -4063,7 +4062,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="64" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A64" s="9" t="s">
         <v>111</v>
       </c>
@@ -4078,7 +4077,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="65" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A65" s="9" t="s">
         <v>109</v>
       </c>
@@ -4093,7 +4092,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="66" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A66" s="9" t="s">
         <v>116</v>
       </c>
@@ -4108,7 +4107,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="67" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A67" s="9" t="s">
         <v>121</v>
       </c>
@@ -4123,7 +4122,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="68" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A68" s="9" t="s">
         <v>96</v>
       </c>
@@ -4138,7 +4137,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="69" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A69" s="9" t="s">
         <v>120</v>
       </c>
@@ -4153,7 +4152,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="70" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A70" s="9" t="s">
         <v>103</v>
       </c>
@@ -4168,7 +4167,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="71" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A71" s="9" t="s">
         <v>115</v>
       </c>
@@ -4183,7 +4182,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="72" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A72" s="9" t="s">
         <v>114</v>
       </c>
@@ -4198,7 +4197,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="73" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A73" s="9" t="s">
         <v>113</v>
       </c>
@@ -4214,7 +4213,7 @@
       </c>
       <c r="F73" s="6"/>
     </row>
-    <row r="74" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A74" s="9" t="s">
         <v>104</v>
       </c>
@@ -4244,7 +4243,7 @@
         <v>Present</v>
       </c>
     </row>
-    <row r="76" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A76" s="9" t="s">
         <v>203</v>
       </c>
@@ -4259,7 +4258,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="77" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A77" s="9" t="s">
         <v>207</v>
       </c>
@@ -4274,7 +4273,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="78" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A78" s="9" t="s">
         <v>209</v>
       </c>
@@ -4289,7 +4288,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="79" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A79" s="9" t="s">
         <v>205</v>
       </c>
@@ -4304,7 +4303,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="80" spans="1:6" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:6" ht="16" x14ac:dyDescent="0.2">
       <c r="A80" s="9" t="s">
         <v>217</v>
       </c>
@@ -4319,7 +4318,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="81" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A81" s="9" t="s">
         <v>219</v>
       </c>
@@ -4334,7 +4333,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="82" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A82" s="3" t="s">
         <v>35</v>
       </c>
@@ -4349,7 +4348,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="83" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A83" s="3" t="s">
         <v>36</v>
       </c>
@@ -4364,7 +4363,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="84" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A84" s="9" t="s">
         <v>112</v>
       </c>
@@ -4379,7 +4378,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="85" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A85" s="9" t="s">
         <v>244</v>
       </c>
@@ -4394,7 +4393,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="86" spans="1:4" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A86" s="3" t="s">
         <v>123</v>
       </c>
@@ -4454,7 +4453,7 @@
         <v>Present</v>
       </c>
     </row>
-    <row r="90" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A90" s="3" t="s">
         <v>15</v>
       </c>
@@ -4469,7 +4468,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="91" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A91" s="7" t="s">
         <v>164</v>
       </c>
@@ -4529,7 +4528,7 @@
         <v>Present</v>
       </c>
     </row>
-    <row r="95" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A95" s="9" t="s">
         <v>101</v>
       </c>
@@ -4574,7 +4573,7 @@
         <v>Present</v>
       </c>
     </row>
-    <row r="98" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A98" s="9" t="s">
         <v>122</v>
       </c>
@@ -4589,7 +4588,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="99" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A99" s="9" t="s">
         <v>107</v>
       </c>
@@ -4604,7 +4603,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="100" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A100" s="9" t="s">
         <v>106</v>
       </c>
@@ -4634,7 +4633,7 @@
         <v>Present</v>
       </c>
     </row>
-    <row r="102" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A102" s="9" t="s">
         <v>245</v>
       </c>
@@ -4649,7 +4648,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="103" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A103" s="9" t="s">
         <v>213</v>
       </c>
@@ -4664,7 +4663,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="104" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A104" s="9" t="s">
         <v>246</v>
       </c>
@@ -4679,7 +4678,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="105" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A105" s="9" t="s">
         <v>231</v>
       </c>
@@ -4694,7 +4693,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="106" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A106" s="9" t="s">
         <v>95</v>
       </c>
@@ -4709,7 +4708,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="107" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A107" s="3" t="s">
         <v>37</v>
       </c>
@@ -4724,7 +4723,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="108" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A108" s="3" t="s">
         <v>38</v>
       </c>
@@ -4739,7 +4738,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="109" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A109" s="3" t="s">
         <v>40</v>
       </c>
@@ -4754,7 +4753,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="110" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A110" s="3" t="s">
         <v>41</v>
       </c>
@@ -4769,7 +4768,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="111" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A111" s="3" t="s">
         <v>39</v>
       </c>
@@ -4784,7 +4783,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="112" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A112" s="9" t="s">
         <v>158</v>
       </c>
@@ -4799,7 +4798,7 @@
         <v>Missing</v>
       </c>
     </row>
-    <row r="113" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A113" s="3" t="s">
         <v>16</v>
       </c>
@@ -4829,7 +4828,7 @@
         <v>Present</v>
       </c>
     </row>
-    <row r="115" spans="1:4" ht="32" hidden="1" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A115" s="7" t="s">
         <v>194</v>
       </c>
@@ -4859,20 +4858,12 @@
         <v>Present</v>
       </c>
     </row>
-    <row r="117" spans="1:4" hidden="1" x14ac:dyDescent="0.2"/>
-    <row r="118" spans="1:4" ht="16" hidden="1" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="B118" s="13" t="s">
         <v>156</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K118" xr:uid="{772E8740-F1F1-5C4E-B137-1D109ADBDF19}">
-    <filterColumn colId="3">
-      <filters>
-        <filter val="Present"/>
-      </filters>
-    </filterColumn>
-  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>